<commit_message>
Update reports with currency formatting
</commit_message>
<xml_diff>
--- a/portfolio_report.xlsx
+++ b/portfolio_report.xlsx
@@ -530,34 +530,50 @@
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>9.92</v>
-      </c>
-      <c r="E2" t="n">
-        <v>991.74</v>
-      </c>
-      <c r="F2" t="n">
-        <v>8.869999999999999</v>
-      </c>
-      <c r="G2" t="n">
-        <v>887</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-104.74</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$9.92</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>$991.74</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>$8.87</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>$887.00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>$-104.74</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>-10.56%</t>
         </is>
       </c>
-      <c r="J2" t="n">
-        <v>34.7</v>
-      </c>
-      <c r="K2" t="n">
-        <v>430.6</v>
-      </c>
-      <c r="L2" t="n">
-        <v>325.86</v>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>$34.70</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>$430.60</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>$325.86</t>
+        </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -592,34 +608,50 @@
           <t>2025-06-27</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>10.97</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1096.54</v>
-      </c>
-      <c r="F3" t="n">
-        <v>11.6</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1159.5</v>
-      </c>
-      <c r="H3" t="n">
-        <v>62.96</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$10.97</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$1,096.54</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>$11.60</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>$1,159.50</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>$62.96</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>5.74%</t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>26.8</v>
-      </c>
-      <c r="K3" t="n">
-        <v>162.6</v>
-      </c>
-      <c r="L3" t="n">
-        <v>225.56</v>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>$26.80</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>$162.60</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>$225.56</t>
+        </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -654,34 +686,50 @@
           <t>2025-05-27</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>13.43</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1343.46</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="G4" t="n">
-        <v>680</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-663.46</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$13.43</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>$1,343.46</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>$6.80</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>$680.00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>$-663.46</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>-49.38%</t>
         </is>
       </c>
-      <c r="J4" t="n">
-        <v>61.4</v>
-      </c>
-      <c r="K4" t="n">
-        <v>761.9</v>
-      </c>
-      <c r="L4" t="n">
-        <v>98.44</v>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>$61.40</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>$761.90</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>$98.44</t>
+        </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -716,34 +764,50 @@
           <t>2025-04-28</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1130.16</v>
-      </c>
-      <c r="F5" t="n">
-        <v>13.69</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1369</v>
-      </c>
-      <c r="H5" t="n">
-        <v>238.84</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$11.30</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$1,130.16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>$13.69</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>$1,369.00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>$238.84</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>21.13%</t>
         </is>
       </c>
-      <c r="J5" t="n">
-        <v>56.9</v>
-      </c>
-      <c r="K5" t="n">
-        <v>469.5</v>
-      </c>
-      <c r="L5" t="n">
-        <v>708.34</v>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>$56.90</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>$469.50</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>$708.34</t>
+        </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -778,34 +842,50 @@
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>10.17</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1017.21</v>
-      </c>
-      <c r="F6" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1458</v>
-      </c>
-      <c r="H6" t="n">
-        <v>440.79</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$10.17</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$1,017.21</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>$14.58</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>$1,458.00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>$440.79</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>43.33%</t>
         </is>
       </c>
-      <c r="J6" t="n">
-        <v>77.59999999999999</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1069.6</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1510.39</v>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>$77.60</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>$1,069.60</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>$1,510.39</t>
+        </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -840,27 +920,51 @@
           <t>2025-03-27</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>56.15</v>
-      </c>
-      <c r="G7" t="n">
-        <v>5615</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>$56.15</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>$5,615.00</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
           <t>nan%</t>
         </is>
       </c>
-      <c r="J7" t="n">
-        <v>177.1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1416.7</v>
-      </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>$177.10</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>$1,358.80</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr">
         <is>
           <t>nan%</t>
@@ -877,7 +981,7 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>2.03</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="8">
@@ -894,52 +998,68 @@
           <t>2025-03-27</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>23.59</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2359.15</v>
-      </c>
-      <c r="F8" t="n">
-        <v>27.87</v>
-      </c>
-      <c r="G8" t="n">
-        <v>2787</v>
-      </c>
-      <c r="H8" t="n">
-        <v>427.85</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$23.99</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>$2,399.35</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>$27.87</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>$2,787.00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>$387.65</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>18.14%</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>180.5</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1772.6</v>
-      </c>
-      <c r="L8" t="n">
-        <v>2200.45</v>
+          <t>16.16%</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>$180.50</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>$1,714.70</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>$2,102.35</t>
+        </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>93.27%</t>
+          <t>87.62%</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>75.14%</t>
+          <t>71.47%</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>161.88%</t>
+          <t>150.76%</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>2.12</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="9">
@@ -956,52 +1076,68 @@
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>78.89</v>
-      </c>
-      <c r="E9" t="n">
-        <v>7889.29</v>
-      </c>
-      <c r="F9" t="n">
-        <v>39.56</v>
-      </c>
-      <c r="G9" t="n">
-        <v>3956</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-3933.29</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$40.75</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>$4,074.60</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>$39.56</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>$3,956.00</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>$-118.60</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>-49.86%</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>26.5</v>
-      </c>
-      <c r="K9" t="n">
-        <v>459.1</v>
-      </c>
-      <c r="L9" t="n">
-        <v>-3474.19</v>
+          <t>-2.91%</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>$265.00</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>$4,501.00</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>$4,382.40</t>
+        </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>-44.04%</t>
+          <t>107.55%</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>5.82%</t>
+          <t>110.46%</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>-49.65%</t>
+          <t>137.06%</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>1.39</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="10">
@@ -1018,27 +1154,51 @@
           <t>2025-04-28</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>24.76</v>
-      </c>
-      <c r="G10" t="n">
-        <v>2475.9</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>$24.76</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>$2,475.90</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
           <t>nan%</t>
         </is>
       </c>
-      <c r="J10" t="n">
-        <v>243.6</v>
-      </c>
-      <c r="K10" t="n">
-        <v>688.5</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>$243.60</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>$688.50</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
           <t>nan%</t>
@@ -1072,34 +1232,50 @@
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>4.94</v>
-      </c>
-      <c r="E11" t="n">
-        <v>493.96</v>
-      </c>
-      <c r="F11" t="n">
-        <v>7.99</v>
-      </c>
-      <c r="G11" t="n">
-        <v>799</v>
-      </c>
-      <c r="H11" t="n">
-        <v>305.04</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$4.94</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>$493.96</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>$7.99</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>$799.00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>$305.04</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
           <t>61.75%</t>
         </is>
       </c>
-      <c r="J11" t="n">
-        <v>55.8</v>
-      </c>
-      <c r="K11" t="n">
-        <v>541.8</v>
-      </c>
-      <c r="L11" t="n">
-        <v>846.84</v>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>$55.80</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>$541.80</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>$846.84</t>
+        </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1134,34 +1310,50 @@
           <t>2025-05-27</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>31.17</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3117.45</v>
-      </c>
-      <c r="F12" t="n">
-        <v>35.95</v>
-      </c>
-      <c r="G12" t="n">
-        <v>3595</v>
-      </c>
-      <c r="H12" t="n">
-        <v>477.55</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$31.17</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>$3,117.45</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>$35.95</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>$3,595.00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>$477.55</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
           <t>15.32%</t>
         </is>
       </c>
-      <c r="J12" t="n">
-        <v>179.2</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1704</v>
-      </c>
-      <c r="L12" t="n">
-        <v>2181.55</v>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>$179.20</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>$1,704.00</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>$2,181.55</t>
+        </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1196,27 +1388,51 @@
           <t>2025-07-28</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>36.75</v>
-      </c>
-      <c r="G13" t="n">
-        <v>3675</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>$36.75</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>$3,675.00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
           <t>nan%</t>
         </is>
       </c>
-      <c r="J13" t="n">
-        <v>245.8</v>
-      </c>
-      <c r="K13" t="n">
-        <v>784.3</v>
-      </c>
-      <c r="L13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>$245.80</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>$784.30</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="M13" t="inlineStr">
         <is>
           <t>nan%</t>
@@ -1250,34 +1466,50 @@
           <t>2025-04-28</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="E14" t="n">
-        <v>920.23</v>
-      </c>
-      <c r="F14" t="n">
-        <v>10.6</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1060</v>
-      </c>
-      <c r="H14" t="n">
-        <v>139.77</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$9.20</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$920.23</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>$10.60</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>$1,060.00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>$139.77</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
           <t>15.19%</t>
         </is>
       </c>
-      <c r="J14" t="n">
-        <v>55.6</v>
-      </c>
-      <c r="K14" t="n">
-        <v>470.2</v>
-      </c>
-      <c r="L14" t="n">
-        <v>609.97</v>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>$55.60</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>$470.20</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>$609.97</t>
+        </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
@@ -1312,52 +1544,68 @@
           <t>2025-08-27</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1330.67</v>
-      </c>
-      <c r="F15" t="n">
-        <v>14.64</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1464</v>
-      </c>
-      <c r="H15" t="n">
-        <v>133.33</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$13.50</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>$1,350.15</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>$14.64</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>$1,464.00</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>$113.85</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>10.02%</t>
-        </is>
-      </c>
-      <c r="J15" t="n">
-        <v>52.3</v>
-      </c>
-      <c r="K15" t="n">
-        <v>223.7</v>
-      </c>
-      <c r="L15" t="n">
-        <v>357.03</v>
+          <t>8.43%</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>$52.30</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>$202.00</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>$315.85</t>
+        </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>26.83%</t>
+          <t>23.39%</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>16.81%</t>
+          <t>14.96%</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>144.73%</t>
+          <t>120.68%</t>
         </is>
       </c>
       <c r="P15" t="n">
-        <v>1.3</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="16">
@@ -1374,52 +1622,68 @@
           <t>2025-05-27</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>36.51</v>
-      </c>
-      <c r="E16" t="n">
-        <v>3651.13</v>
-      </c>
-      <c r="F16" t="n">
-        <v>44.21</v>
-      </c>
-      <c r="G16" t="n">
-        <v>4421</v>
-      </c>
-      <c r="H16" t="n">
-        <v>769.87</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$36.87</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>$3,687.21</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>$44.21</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>$4,421.00</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>$733.79</t>
+        </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>21.09%</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>126.6</v>
-      </c>
-      <c r="K16" t="n">
-        <v>902.6</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1672.47</v>
+          <t>19.9%</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>$126.60</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>$857.00</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>$1,590.79</t>
+        </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>45.81%</t>
+          <t>43.14%</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>24.72%</t>
+          <t>23.24%</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>107.26%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="P16" t="n">
-        <v>1.8</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="17">
@@ -1436,27 +1700,51 @@
           <t>2025-02-27</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>38.2</v>
-      </c>
-      <c r="G17" t="n">
-        <v>3820</v>
-      </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>$38.20</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>$3,820.00</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr">
         <is>
           <t>nan%</t>
         </is>
       </c>
-      <c r="J17" t="n">
-        <v>333</v>
-      </c>
-      <c r="K17" t="n">
-        <v>2080</v>
-      </c>
-      <c r="L17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>$333.00</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>$2,080.00</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>$nan</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr">
         <is>
           <t>nan%</t>
@@ -1490,34 +1778,50 @@
           <t>2025-07-28</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>16.32</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1632</v>
-      </c>
-      <c r="F18" t="n">
-        <v>15.85</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1585</v>
-      </c>
-      <c r="H18" t="n">
-        <v>-47</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$16.32</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>$1,632.00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>$15.85</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>$1,585.00</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>$-47.00</t>
+        </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
           <t>-2.88%</t>
         </is>
       </c>
-      <c r="J18" t="n">
-        <v>44.4</v>
-      </c>
-      <c r="K18" t="n">
-        <v>154</v>
-      </c>
-      <c r="L18" t="n">
-        <v>107</v>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>$44.40</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>$154.00</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>$107.00</t>
+        </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
@@ -1552,34 +1856,50 @@
           <t>2025-06-27</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>11.27</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1126.54</v>
-      </c>
-      <c r="F19" t="n">
-        <v>14.89</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1489</v>
-      </c>
-      <c r="H19" t="n">
-        <v>362.46</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$11.27</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>$1,126.54</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>$14.89</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>$1,489.00</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>$362.46</t>
+        </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
           <t>32.17%</t>
         </is>
       </c>
-      <c r="J19" t="n">
-        <v>55.3</v>
-      </c>
-      <c r="K19" t="n">
-        <v>507.5</v>
-      </c>
-      <c r="L19" t="n">
-        <v>869.96</v>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>$55.30</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>$507.50</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>$869.96</t>
+        </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
@@ -1614,34 +1934,50 @@
           <t>2025-07-28</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>51.01</v>
-      </c>
-      <c r="E20" t="n">
-        <v>5100.56</v>
-      </c>
-      <c r="F20" t="n">
-        <v>53.43</v>
-      </c>
-      <c r="G20" t="n">
-        <v>5343</v>
-      </c>
-      <c r="H20" t="n">
-        <v>242.44</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$51.01</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>$5,100.56</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>$53.43</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>$5,343.00</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>$242.44</t>
+        </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
           <t>4.75%</t>
         </is>
       </c>
-      <c r="J20" t="n">
-        <v>370.6</v>
-      </c>
-      <c r="K20" t="n">
-        <v>1944.6</v>
-      </c>
-      <c r="L20" t="n">
-        <v>2187.04</v>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>$370.60</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>$1,944.60</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>$2,187.04</t>
+        </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
@@ -1676,34 +2012,50 @@
           <t>2025-07-28</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>15</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1500.27</v>
-      </c>
-      <c r="F21" t="n">
-        <v>9.859999999999999</v>
-      </c>
-      <c r="G21" t="n">
-        <v>986</v>
-      </c>
-      <c r="H21" t="n">
-        <v>-514.27</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>$15.00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>$1,500.27</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>$9.86</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>$986.00</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>$-514.27</t>
+        </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
           <t>-34.28%</t>
         </is>
       </c>
-      <c r="J21" t="n">
-        <v>96.90000000000001</v>
-      </c>
-      <c r="K21" t="n">
-        <v>549.3</v>
-      </c>
-      <c r="L21" t="n">
-        <v>35.03</v>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>$96.90</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>$549.30</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>$35.03</t>
+        </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
@@ -1738,34 +2090,50 @@
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>29.99</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2998.51</v>
-      </c>
-      <c r="F22" t="n">
-        <v>53.01</v>
-      </c>
-      <c r="G22" t="n">
-        <v>5301</v>
-      </c>
-      <c r="H22" t="n">
-        <v>2302.49</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>$29.99</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>$2,998.51</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>$53.01</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>$5,301.00</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>$2,302.49</t>
+        </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
           <t>76.79%</t>
         </is>
       </c>
-      <c r="J22" t="n">
-        <v>337.5</v>
-      </c>
-      <c r="K22" t="n">
-        <v>5108.4</v>
-      </c>
-      <c r="L22" t="n">
-        <v>7410.89</v>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>$337.50</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>$5,108.40</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>$7,410.89</t>
+        </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
@@ -1800,34 +2168,50 @@
           <t>2025-07-28</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>7.49</v>
-      </c>
-      <c r="E23" t="n">
-        <v>748.8</v>
-      </c>
-      <c r="F23" t="n">
-        <v>7.46</v>
-      </c>
-      <c r="G23" t="n">
-        <v>746</v>
-      </c>
-      <c r="H23" t="n">
-        <v>-2.8</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>$7.49</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>$748.80</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>$7.46</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>$746.00</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>$-2.80</t>
+        </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
           <t>-0.37%</t>
         </is>
       </c>
-      <c r="J23" t="n">
-        <v>30.3</v>
-      </c>
-      <c r="K23" t="n">
-        <v>176.4</v>
-      </c>
-      <c r="L23" t="n">
-        <v>173.6</v>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>$30.30</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>$176.40</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>$173.60</t>
+        </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
@@ -1862,34 +2246,50 @@
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="D24" t="n">
-        <v>6.04</v>
-      </c>
-      <c r="E24" t="n">
-        <v>603.88</v>
-      </c>
-      <c r="F24" t="n">
-        <v>4.58</v>
-      </c>
-      <c r="G24" t="n">
-        <v>458</v>
-      </c>
-      <c r="H24" t="n">
-        <v>-145.88</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>$6.04</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>$603.88</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>$4.58</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>$458.00</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>$-145.88</t>
+        </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>-24.16%</t>
         </is>
       </c>
-      <c r="J24" t="n">
-        <v>30.2</v>
-      </c>
-      <c r="K24" t="n">
-        <v>647.2</v>
-      </c>
-      <c r="L24" t="n">
-        <v>501.32</v>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>$30.20</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>$647.20</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>$501.32</t>
+        </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>

</xml_diff>